<commit_message>
update, and also worked on documents and datasets sorted by types
</commit_message>
<xml_diff>
--- a/metadata/rbk1/Nitro1843/BroadbalkSoilNdata.xlsx
+++ b/metadata/rbk1/Nitro1843/BroadbalkSoilNdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rothamsted.sharepoint.com/sites/e-RA/Shared Documents/Data-docs repository/metadata/rbk1/Nitro1843/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_3395889E9B5C9687CC92075085C1F12AA6E012AD" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B1300DB6-BB0E-499D-B683-09F5A49595E5}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="11_3395889E9B5C9687CC92075085C1F12AA6E012AD" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4FF946D9-F744-48C2-BD43-B25D939BE208}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="-12585" windowWidth="18510" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1710" yWindow="-14760" windowWidth="18510" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Soil N data" sheetId="6" r:id="rId1"/>
@@ -332,9 +332,6 @@
     <t>Data for 1966 and 1987 are by Kjeldahl analysis for Total N.</t>
   </si>
   <si>
-    <t>Data for 1992, 1997, 2000, 2005 and 2010 are by combustion (LECO)</t>
-  </si>
-  <si>
     <t>Data for 1865 are original Soda Lime analyses (from Dyer, 1902) corrected to be equivalent to LECO</t>
   </si>
   <si>
@@ -414,6 +411,9 @@
   </si>
   <si>
     <t>Values in red are estimated (see notes below).</t>
+  </si>
+  <si>
+    <t>Data for 1992, 1997, 2000, 2005 and 2010 are Total N by combustion (LECO)</t>
   </si>
 </sst>
 </file>
@@ -946,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,7 +1023,7 @@
   <sheetData>
     <row r="1" spans="2:17" ht="21" x14ac:dyDescent="0.3">
       <c r="B1" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1073,7 +1073,7 @@
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="8" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
@@ -1155,7 +1155,7 @@
         <v>17</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>1</v>
@@ -1655,17 +1655,17 @@
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
@@ -1675,7 +1675,7 @@
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="2:7" ht="17.25" x14ac:dyDescent="0.25">
@@ -1685,7 +1685,7 @@
     </row>
     <row r="37" spans="2:7" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="2:7" ht="17.25" x14ac:dyDescent="0.25">
@@ -1710,12 +1710,12 @@
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
@@ -1725,7 +1725,7 @@
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
@@ -1734,7 +1734,7 @@
       </c>
       <c r="D48" s="14"/>
       <c r="G48" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1747,6 +1747,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100622C72A1DD75CA4D87E39FE37B04C3D3" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a181992610faed44b90126dc36e4bac8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6584b4ba-af75-4ac8-8379-7172592f8823" xmlns:ns3="a9e4a452-7199-439f-b4c2-3c6fe4528eb3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eb744a54a586913629e94f53228026f2" ns2:_="" ns3:_="">
     <xsd:import namespace="6584b4ba-af75-4ac8-8379-7172592f8823"/>
@@ -1963,12 +1969,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1979,6 +1979,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ACD4C3B-CAD2-4989-8E10-C65298BCD755}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21039941-7F28-4312-B623-6AE619D3C42F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1997,15 +2006,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ACD4C3B-CAD2-4989-8E10-C65298BCD755}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD9E8237-3A08-459A-A8FA-604AB370399A}">
   <ds:schemaRefs>

</xml_diff>